<commit_message>
RTTBC23 Week 7 (Hon Miss) Entries Posted
</commit_message>
<xml_diff>
--- a/pdf/RTTBC23-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC23-Schedule-by-Division.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1034" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A5A9812-E7BE-459A-A7C8-866C461DF21B}"/>
+  <xr:revisionPtr revIDLastSave="1036" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDB1D8C5-181F-43CF-8954-20E21F4AED09}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
@@ -750,129 +750,178 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -881,55 +930,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1258,12 +1258,12 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I28" sqref="I28:I30"/>
+      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="4.21875" style="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.21875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1274,124 +1274,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="27" t="s">
+      <c r="A1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="67" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="35" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="22"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="68" t="s">
+      <c r="A3" s="69"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="22"/>
-      <c r="B4" s="78">
+      <c r="A4" s="69"/>
+      <c r="B4" s="56">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="42" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="24"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="22"/>
-      <c r="B5" s="79"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="46" t="s">
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
-      <c r="B6" s="80"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="26"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="22"/>
-      <c r="B7" s="81">
+      <c r="A7" s="69"/>
+      <c r="B7" s="39">
         <v>2</v>
       </c>
       <c r="C7" s="5"/>
@@ -1407,8 +1407,8 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="22"/>
-      <c r="B8" s="81">
+      <c r="A8" s="69"/>
+      <c r="B8" s="39">
         <v>3</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -1424,22 +1424,22 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
-      <c r="B9" s="78">
+      <c r="A9" s="69"/>
+      <c r="B9" s="56">
         <v>4</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="33" t="s">
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="41" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="7" t="s">
@@ -1447,23 +1447,23 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="43"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="66" t="s">
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="78">
+      <c r="A11" s="69"/>
+      <c r="B11" s="56">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1472,47 +1472,47 @@
       <c r="D11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="33" t="s">
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="24"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="22"/>
-      <c r="B12" s="79"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="25"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="22"/>
-      <c r="B13" s="80"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="26"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="44"/>
     </row>
     <row r="14" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="22"/>
-      <c r="B14" s="81">
+      <c r="A14" s="69"/>
+      <c r="B14" s="39">
         <v>6</v>
       </c>
       <c r="C14" s="5"/>
@@ -1528,308 +1528,308 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="22"/>
-      <c r="B15" s="78">
+      <c r="A15" s="69"/>
+      <c r="B15" s="56">
         <v>7</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="35" t="s">
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="43"/>
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="22"/>
-      <c r="B16" s="79"/>
-      <c r="C16" s="44" t="s">
+      <c r="A16" s="69"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="25"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="52"/>
     </row>
     <row r="17" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="22"/>
-      <c r="B17" s="80"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="26"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="44"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
-      <c r="B18" s="78">
+      <c r="A18" s="69"/>
+      <c r="B18" s="56">
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
       <c r="I18" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="22"/>
-      <c r="B19" s="79"/>
-      <c r="C19" s="49" t="s">
+      <c r="A19" s="69"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="46" t="s">
+      <c r="D19" s="49"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="22"/>
-      <c r="B20" s="80"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="47" t="s">
+      <c r="D20" s="50"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A21" s="22"/>
-      <c r="B21" s="78">
+      <c r="A21" s="69"/>
+      <c r="B21" s="56">
         <v>9</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="33" t="s">
+      <c r="E21" s="43"/>
+      <c r="F21" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="43"/>
+      <c r="H21" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="24"/>
+      <c r="I21" s="43"/>
     </row>
     <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="79"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="25"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="52"/>
     </row>
     <row r="23" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="22"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="26"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="44"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="22"/>
-      <c r="B24" s="78">
+      <c r="A24" s="69"/>
+      <c r="B24" s="56">
         <v>10</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
     </row>
     <row r="25" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
-      <c r="B25" s="80"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
       <c r="E25" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
     </row>
     <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="78">
+      <c r="A26" s="69"/>
+      <c r="B26" s="56">
         <v>11</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="D26" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
     </row>
     <row r="27" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="22"/>
-      <c r="B27" s="80"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
     </row>
     <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="22"/>
-      <c r="B28" s="78">
+      <c r="A28" s="69"/>
+      <c r="B28" s="56">
         <v>12</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="53" t="s">
+      <c r="D28" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="48" t="s">
+      <c r="E28" s="43"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="45" t="s">
+      <c r="H28" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="24"/>
+      <c r="I28" s="43"/>
     </row>
     <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A29" s="22"/>
-      <c r="B29" s="79"/>
-      <c r="C29" s="46" t="s">
+      <c r="A29" s="69"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="55"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="46" t="s">
+      <c r="D29" s="46"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="24" t="s">
         <v>62</v>
       </c>
       <c r="H29" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="25"/>
+      <c r="I29" s="52"/>
     </row>
     <row r="30" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="22"/>
-      <c r="B30" s="80"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="58"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="30"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="55"/>
       <c r="G30" s="17" t="s">
         <v>66</v>
       </c>
       <c r="H30" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="26"/>
+      <c r="I30" s="44"/>
     </row>
     <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A31" s="22"/>
-      <c r="B31" s="78">
+      <c r="A31" s="69"/>
+      <c r="B31" s="56">
         <v>13</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="53" t="s">
+      <c r="E31" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="F31" s="57" t="s">
+      <c r="F31" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="24"/>
-      <c r="H31" s="35" t="s">
+      <c r="G31" s="43"/>
+      <c r="H31" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="I31" s="24"/>
+      <c r="I31" s="43"/>
     </row>
     <row r="32" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="22"/>
-      <c r="B32" s="80"/>
-      <c r="C32" s="47" t="s">
+      <c r="A32" s="69"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="26"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="44"/>
     </row>
     <row r="33" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="22"/>
-      <c r="B33" s="81">
+      <c r="A33" s="69"/>
+      <c r="B33" s="39">
         <v>14</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="59" t="s">
+      <c r="E33" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="60" t="s">
+      <c r="F33" s="31" t="s">
         <v>73</v>
       </c>
       <c r="G33" s="6"/>
@@ -1837,18 +1837,18 @@
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="22"/>
-      <c r="B34" s="81">
+      <c r="A34" s="69"/>
+      <c r="B34" s="39">
         <v>15</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="61" t="s">
+      <c r="E34" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="62" t="s">
+      <c r="F34" s="33" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="6"/>
@@ -1856,68 +1856,68 @@
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A35" s="22"/>
-      <c r="B35" s="78">
+      <c r="A35" s="69"/>
+      <c r="B35" s="56">
         <v>16</v>
       </c>
-      <c r="C35" s="48" t="s">
+      <c r="C35" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="48" t="s">
+      <c r="D35" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="33" t="s">
+      <c r="E35" s="53"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="I35" s="35" t="s">
+      <c r="I35" s="41" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
-      <c r="B36" s="79"/>
+      <c r="A36" s="69"/>
+      <c r="B36" s="57"/>
       <c r="C36" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="36"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="51"/>
     </row>
     <row r="37" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
-      <c r="B37" s="80"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="15" t="s">
         <v>84</v>
       </c>
       <c r="D37" s="4"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="37"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="22"/>
-      <c r="B38" s="78">
+      <c r="A38" s="69"/>
+      <c r="B38" s="56">
         <v>17</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="63" t="s">
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="80" t="s">
         <v>92</v>
       </c>
       <c r="H38" s="10" t="s">
@@ -1928,108 +1928,108 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A39" s="22"/>
-      <c r="B39" s="79"/>
-      <c r="C39" s="44" t="s">
+      <c r="A39" s="69"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="64"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="81"/>
       <c r="H39" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="I39" s="49" t="s">
+      <c r="I39" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="22"/>
-      <c r="B40" s="79"/>
+      <c r="A40" s="69"/>
+      <c r="B40" s="57"/>
       <c r="C40" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="56"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="64"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="81"/>
       <c r="H40" s="14" t="s">
         <v>89</v>
       </c>
       <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="22"/>
-      <c r="B41" s="80"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="58"/>
       <c r="C41" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D41" s="40"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="65"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="82"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A42" s="22"/>
-      <c r="B42" s="78">
+      <c r="A42" s="69"/>
+      <c r="B42" s="56">
         <v>18</v>
       </c>
-      <c r="C42" s="24"/>
+      <c r="C42" s="43"/>
       <c r="D42" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E42" s="45" t="s">
+      <c r="E42" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="F42" s="45" t="s">
+      <c r="F42" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="G42" s="24"/>
-      <c r="H42" s="31" t="s">
+      <c r="G42" s="43"/>
+      <c r="H42" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="62" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A43" s="22"/>
-      <c r="B43" s="79"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="44" t="s">
+      <c r="A43" s="69"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="E43" s="44" t="s">
+      <c r="E43" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="F43" s="44" t="s">
+      <c r="F43" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="G43" s="25"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
     </row>
     <row r="44" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="22"/>
-      <c r="B44" s="80"/>
-      <c r="C44" s="26"/>
+      <c r="A44" s="69"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="44"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="47" t="s">
+      <c r="E44" s="25" t="s">
         <v>102</v>
       </c>
       <c r="F44" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G44" s="26"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
     </row>
     <row r="45" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="22"/>
-      <c r="B45" s="81">
+      <c r="A45" s="69"/>
+      <c r="B45" s="39">
         <v>20</v>
       </c>
       <c r="C45" s="6"/>
@@ -2043,20 +2043,20 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="23"/>
-      <c r="B46" s="69" t="s">
+      <c r="A46" s="70"/>
+      <c r="B46" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="69"/>
-      <c r="I46" s="70"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="76"/>
     </row>
     <row r="47" spans="1:9" s="19" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="23"/>
+      <c r="A47" s="70"/>
       <c r="B47" s="21"/>
       <c r="C47" s="20">
         <f t="shared" ref="C47:I47" si="0">COUNTIF(C4:C45, "&lt;&gt;")</f>
@@ -2088,21 +2088,21 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="23"/>
-      <c r="B48" s="69" t="str">
+      <c r="A48" s="70"/>
+      <c r="B48" s="65" t="str">
         <f>SUM(C47:I47) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>102 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C48" s="69"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="69"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="69"/>
-      <c r="I48" s="69"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="65"/>
+      <c r="I48" s="65"/>
     </row>
     <row r="49" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="23"/>
+      <c r="A49" s="70"/>
       <c r="B49" s="71" t="s">
         <v>114</v>
       </c>
@@ -2118,21 +2118,52 @@
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="I35:I37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="A2:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
     <mergeCell ref="H42:H44"/>
     <mergeCell ref="I42:I44"/>
     <mergeCell ref="B48:I48"/>
@@ -2149,6 +2180,13 @@
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="E28:E30"/>
     <mergeCell ref="I24:I25"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="D26:D27"/>
@@ -2158,59 +2196,21 @@
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A2:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="F38:F41"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="E35:E37"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" fitToHeight="10" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;20Road to the Breeders' Cup '23 Schedule by Division</oddHeader>
-    <oddFooter>&amp;L&amp;14Gallop Racing LLC</oddFooter>
+    <oddFooter>&amp;C&amp;14Gallop Racing LLC</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GRCW-691; RTTBC23 Week 17 Noms (CD)
</commit_message>
<xml_diff>
--- a/pdf/RTTBC23-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC23-Schedule-by-Division.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1038" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87093F86-4D41-4E8E-B163-121B22850CAE}"/>
+  <xr:revisionPtr revIDLastSave="1044" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56D59138-F583-43D7-8A08-11CAD3744A31}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
@@ -526,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -590,37 +590,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -689,52 +658,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -747,28 +713,28 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -783,23 +749,113 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -808,21 +864,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -838,20 +879,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -862,74 +906,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1258,12 +1236,12 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H35" sqref="H35:H37"/>
+      <selection pane="bottomLeft" activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="4.21875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.21875" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1274,456 +1252,456 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="61" t="s">
+      <c r="A1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="34" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="33" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="40"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="35" t="s">
+      <c r="A3" s="69"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="40"/>
-      <c r="B4" s="45">
+      <c r="A4" s="69"/>
+      <c r="B4" s="56">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="65" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="43"/>
+      <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="40"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="69"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="23" t="s">
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="69"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="44"/>
       <c r="F6" s="44"/>
-      <c r="G6" s="66"/>
+      <c r="G6" s="61"/>
       <c r="H6" s="44"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="40"/>
-      <c r="B7" s="38">
+      <c r="A7" s="69"/>
+      <c r="B7" s="37">
         <v>2</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="12" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="40"/>
-      <c r="B8" s="38">
+      <c r="A8" s="69"/>
+      <c r="B8" s="37">
         <v>3</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="12" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
-      <c r="B9" s="45">
+      <c r="A9" s="69"/>
+      <c r="B9" s="56">
         <v>4</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="62" t="s">
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="14" t="s">
+      <c r="A10" s="69"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="13" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="44"/>
       <c r="F10" s="44"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="33" t="s">
+      <c r="G10" s="50"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="32" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="45">
+      <c r="A11" s="69"/>
+      <c r="B11" s="56">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="62" t="s">
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="42"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="11" t="s">
+      <c r="A12" s="69"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="43"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="69"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="44"/>
       <c r="F13" s="44"/>
       <c r="G13" s="44"/>
-      <c r="H13" s="64"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="44"/>
     </row>
     <row r="14" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="40"/>
-      <c r="B14" s="38">
+      <c r="A14" s="69"/>
+      <c r="B14" s="37">
         <v>6</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="12" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="40"/>
-      <c r="B15" s="45">
+      <c r="A15" s="69"/>
+      <c r="B15" s="56">
         <v>7</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="67" t="s">
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="42"/>
+      <c r="I15" s="43"/>
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="40"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="21" t="s">
+      <c r="A16" s="69"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="43"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="52"/>
     </row>
     <row r="17" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="40"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="14" t="s">
+      <c r="A17" s="69"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="44"/>
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
-      <c r="H17" s="68"/>
+      <c r="H17" s="42"/>
       <c r="I17" s="44"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="40"/>
-      <c r="B18" s="45">
+      <c r="A18" s="69"/>
+      <c r="B18" s="56">
         <v>8</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="62" t="s">
+      <c r="D18" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="7" t="s">
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="40"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="26" t="s">
+      <c r="A19" s="69"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="63"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="23" t="s">
+      <c r="D19" s="49"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="40"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="64"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="44"/>
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
       <c r="H20" s="44"/>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A21" s="40"/>
-      <c r="B21" s="45">
+      <c r="A21" s="69"/>
+      <c r="B21" s="56">
         <v>9</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="62" t="s">
+      <c r="E21" s="43"/>
+      <c r="F21" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="69" t="s">
+      <c r="G21" s="43"/>
+      <c r="H21" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="42"/>
+      <c r="I21" s="43"/>
     </row>
     <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="8" t="s">
+      <c r="A22" s="69"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="78"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="43"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="52"/>
     </row>
     <row r="23" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="40"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="14" t="s">
+      <c r="A23" s="69"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="66"/>
+      <c r="D23" s="61"/>
       <c r="E23" s="44"/>
-      <c r="F23" s="64"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="44"/>
-      <c r="H23" s="71"/>
+      <c r="H23" s="47"/>
       <c r="I23" s="44"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="40"/>
-      <c r="B24" s="45">
+      <c r="A24" s="69"/>
+      <c r="B24" s="56">
         <v>10</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="7" t="s">
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="62" t="s">
+      <c r="F24" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
     </row>
     <row r="25" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="40"/>
-      <c r="B25" s="46"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="44"/>
       <c r="D25" s="44"/>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="64"/>
+      <c r="F25" s="50"/>
       <c r="G25" s="44"/>
       <c r="H25" s="44"/>
       <c r="I25" s="44"/>
     </row>
     <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
-      <c r="B26" s="45">
+      <c r="A26" s="69"/>
+      <c r="B26" s="56">
         <v>11</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="69" t="s">
+      <c r="D26" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
     </row>
     <row r="27" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="40"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="14" t="s">
+      <c r="A27" s="69"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="71"/>
+      <c r="D27" s="47"/>
       <c r="E27" s="44"/>
       <c r="F27" s="44"/>
       <c r="G27" s="44"/>
@@ -1731,401 +1709,456 @@
       <c r="I27" s="44"/>
     </row>
     <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="40"/>
-      <c r="B28" s="45">
+      <c r="A28" s="69"/>
+      <c r="B28" s="56">
         <v>12</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="69" t="s">
+      <c r="D28" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="25" t="s">
+      <c r="E28" s="43"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="42"/>
+      <c r="I28" s="43"/>
     </row>
     <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A29" s="40"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="23" t="s">
+      <c r="A29" s="69"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="23" t="s">
+      <c r="D29" s="46"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="43"/>
+      <c r="I29" s="52"/>
     </row>
     <row r="30" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="40"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="71"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="44"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="16" t="s">
+      <c r="F30" s="55"/>
+      <c r="G30" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="13" t="s">
         <v>59</v>
       </c>
       <c r="I30" s="44"/>
     </row>
     <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A31" s="40"/>
-      <c r="B31" s="45">
+      <c r="A31" s="69"/>
+      <c r="B31" s="56">
         <v>13</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="62" t="s">
+      <c r="D31" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="69" t="s">
+      <c r="E31" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="F31" s="76" t="s">
+      <c r="F31" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="42"/>
-      <c r="H31" s="67" t="s">
+      <c r="G31" s="43"/>
+      <c r="H31" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="I31" s="42"/>
+      <c r="I31" s="43"/>
     </row>
     <row r="32" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="40"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="24" t="s">
+      <c r="A32" s="69"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="77"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="67"/>
       <c r="G32" s="44"/>
-      <c r="H32" s="68"/>
+      <c r="H32" s="42"/>
       <c r="I32" s="44"/>
     </row>
     <row r="33" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="40"/>
-      <c r="B33" s="38">
+      <c r="A33" s="69"/>
+      <c r="B33" s="37">
         <v>14</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="29" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="40"/>
-      <c r="B34" s="38">
+      <c r="A34" s="69"/>
+      <c r="B34" s="37">
         <v>15</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="12" t="s">
+      <c r="C34" s="5"/>
+      <c r="D34" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="32" t="s">
+      <c r="F34" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A35" s="40"/>
-      <c r="B35" s="45">
+      <c r="A35" s="69"/>
+      <c r="B35" s="56">
         <v>16</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="79"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="62" t="s">
+      <c r="E35" s="53"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="I35" s="67" t="s">
+      <c r="I35" s="41" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="40"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="8" t="s">
+      <c r="A36" s="69"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="80"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="72"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="51"/>
     </row>
     <row r="37" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="40"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="14" t="s">
+      <c r="A37" s="69"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="81"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="44"/>
       <c r="G37" s="44"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="68"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="40"/>
-      <c r="B38" s="45">
+      <c r="A38" s="69"/>
+      <c r="B38" s="56">
         <v>17</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="54" t="s">
+      <c r="D38" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="57" t="s">
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A39" s="40"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="21" t="s">
+      <c r="A39" s="69"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="55"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="11" t="s">
+      <c r="D39" s="78"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="I39" s="26" t="s">
+      <c r="I39" s="25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="40"/>
-      <c r="B40" s="60"/>
-      <c r="C40" s="11" t="s">
+      <c r="A40" s="69"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="55"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="82" t="s">
-        <v>119</v>
-      </c>
-      <c r="I40" s="2"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
     </row>
     <row r="41" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="40"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="14" t="s">
+      <c r="A41" s="69"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="56"/>
+      <c r="D41" s="79"/>
       <c r="E41" s="44"/>
       <c r="F41" s="44"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
     </row>
     <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A42" s="40"/>
-      <c r="B42" s="45">
+      <c r="A42" s="69"/>
+      <c r="B42" s="56">
         <v>18</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="7" t="s">
+      <c r="C42" s="43"/>
+      <c r="D42" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="F42" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="G42" s="42"/>
-      <c r="H42" s="73" t="s">
+      <c r="G42" s="43"/>
+      <c r="H42" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="I42" s="73" t="s">
+      <c r="I42" s="62" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A43" s="40"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="21" t="s">
+      <c r="A43" s="69"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43" s="63"/>
     </row>
     <row r="44" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="40"/>
-      <c r="B44" s="46"/>
+      <c r="A44" s="69"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="44"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="24" t="s">
+      <c r="D44" s="3"/>
+      <c r="E44" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="F44" s="15" t="s">
         <v>100</v>
       </c>
       <c r="G44" s="44"/>
-      <c r="H44" s="75"/>
-      <c r="I44" s="75"/>
+      <c r="H44" s="85"/>
+      <c r="I44" s="64"/>
     </row>
     <row r="45" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="40"/>
-      <c r="B45" s="38">
+      <c r="A45" s="69"/>
+      <c r="B45" s="37">
         <v>20</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="17" t="s">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="I45" s="6"/>
+      <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="41"/>
-      <c r="B46" s="52" t="s">
+      <c r="A46" s="70"/>
+      <c r="B46" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="52"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="53"/>
-    </row>
-    <row r="47" spans="1:9" s="18" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="41"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="19">
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="76"/>
+    </row>
+    <row r="47" spans="1:9" s="17" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="70"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="18">
         <f t="shared" ref="C47:I47" si="0">COUNTIF(C4:C45, "&lt;&gt;")</f>
         <v>29</v>
       </c>
-      <c r="D47" s="19">
+      <c r="D47" s="18">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E47" s="19">
+      <c r="E47" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F47" s="19">
+      <c r="F47" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G47" s="19">
+      <c r="G47" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H47" s="19">
+      <c r="H47" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I47" s="19">
+      <c r="I47" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="41"/>
-      <c r="B48" s="52" t="str">
+      <c r="A48" s="70"/>
+      <c r="B48" s="65" t="str">
         <f>SUM(C47:I47) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>102 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="65"/>
+      <c r="I48" s="65"/>
     </row>
     <row r="49" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="41"/>
-      <c r="B49" s="47" t="s">
+      <c r="A49" s="70"/>
+      <c r="B49" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="49" t="s">
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="51"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="74"/>
+      <c r="I49" s="75"/>
     </row>
   </sheetData>
-  <mergeCells count="86">
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="I35:I37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="E35:E37"/>
+  <mergeCells count="87">
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="A2:A45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B11:B13"/>
@@ -2142,68 +2175,14 @@
     <mergeCell ref="H26:H27"/>
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A2:A45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="F38:F41"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="E35:E37"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>